<commit_message>
added checking of completeness
</commit_message>
<xml_diff>
--- a/docs/tutorial/use-cases/spreadsheets/information-architect-david.xlsx
+++ b/docs/tutorial/use-cases/spreadsheets/information-architect-david.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Secondary/repos/neat/docs/tutorial/use-cases/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDD5B1A-C5D8-F443-A7F0-A0ABF7386F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99EB29CD-5016-9346-9F46-A559D4A1E074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="32380" windowHeight="26540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="107">
   <si>
     <t>Data model classes</t>
   </si>
@@ -622,6 +622,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -631,8 +633,6 @@
     <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -941,7 +941,7 @@
   <dimension ref="A1:W1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -967,10 +967,10 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="17.25" customHeight="1">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="30" t="s">
         <v>106</v>
       </c>
     </row>
@@ -8813,7 +8813,7 @@
   <dimension ref="A1:Z954"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8831,18 +8831,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="37.5" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -15099,7 +15099,9 @@
   </sheetPr>
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:A25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -15111,13 +15113,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="37.5" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -15330,11 +15332,31 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1"/>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1"/>
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A25" t="s">
+        <v>72</v>
+      </c>
+    </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="27" spans="1:4" ht="15.75" customHeight="1"/>
     <row r="28" spans="1:4" ht="15.75" customHeight="1"/>

</xml_diff>